<commit_message>
Correction of data file format and other smal changes
</commit_message>
<xml_diff>
--- a/MarkVdata.xlsx
+++ b/MarkVdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\MarkV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proj\MarkV\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6752A2F6-E0FA-44AB-B469-9C3FEFFD17EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="1000" activeTab="4"/>
+    <workbookView xWindow="8952" yWindow="1272" windowWidth="18564" windowHeight="13932" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Пути" sheetId="5" r:id="rId1"/>
@@ -210,9 +211,6 @@
     <t>.\man\Справка.pdf</t>
   </si>
   <si>
-    <t>(проводники)</t>
-  </si>
-  <si>
     <t>(кабели)</t>
   </si>
   <si>
@@ -349,12 +347,15 @@
   </si>
   <si>
     <t>https://catalog.weidmueller.com/catalog/Start.do?localeId=en&amp;ObjectID=2539390000</t>
+  </si>
+  <si>
+    <t>(провода)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,30 +422,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="№"/>
-    <tableColumn id="2" name="Вид"/>
-    <tableColumn id="3" name="Наименование"/>
-    <tableColumn id="6" name="Материал"/>
-    <tableColumn id="4" name="Крепление"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Вид"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Наименование"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Материал"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Крепление"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:G15" totalsRowShown="0">
-  <autoFilter ref="A1:G15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Таблица3" displayName="Таблица3" ref="A1:G15" totalsRowShown="0">
+  <autoFilter ref="A1:G15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Вид"/>
-    <tableColumn id="2" name="Производитель"/>
-    <tableColumn id="3" name="Артикул"/>
-    <tableColumn id="4" name="Тип"/>
-    <tableColumn id="5" name="Примечание"/>
-    <tableColumn id="6" name="Файл"/>
-    <tableColumn id="7" name="WEB-адрес"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Вид"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Производитель"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Артикул"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Тип"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Примечание"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Файл"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="WEB-адрес"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,7 +713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -723,10 +724,10 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -760,7 +761,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -771,14 +772,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -897,19 +898,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -937,13 +939,13 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1020,7 +1022,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Лист4"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1031,11 +1033,11 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1110,25 +1112,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="140.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="140.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1136,38 +1138,38 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>48</v>
       </c>
       <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
-      </c>
-      <c r="G1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1176,21 +1178,21 @@
         <v>1513250000</v>
       </c>
       <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
         <v>71</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
         <v>72</v>
-      </c>
-      <c r="F3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1199,21 +1201,21 @@
         <v>1513270000</v>
       </c>
       <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
         <v>74</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
         <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1222,21 +1224,21 @@
         <v>1513290000</v>
       </c>
       <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
         <v>77</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
         <v>78</v>
-      </c>
-      <c r="F5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1245,16 +1247,16 @@
         <v>1513320000</v>
       </c>
       <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
         <v>80</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
         <v>81</v>
-      </c>
-      <c r="F6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1268,10 +1270,10 @@
         <v>1609801044</v>
       </c>
       <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
         <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1285,15 +1287,15 @@
         <v>1059780000</v>
       </c>
       <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" t="s">
         <v>85</v>
-      </c>
-      <c r="F8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -1302,15 +1304,15 @@
         <v>2005500000</v>
       </c>
       <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
         <v>88</v>
-      </c>
-      <c r="F9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1319,15 +1321,15 @@
         <v>2006140000</v>
       </c>
       <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
         <v>91</v>
-      </c>
-      <c r="F10" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -1336,15 +1338,15 @@
         <v>1327830000</v>
       </c>
       <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" t="s">
         <v>94</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1353,10 +1355,10 @@
         <v>1327800000</v>
       </c>
       <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" t="s">
         <v>97</v>
-      </c>
-      <c r="F12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1370,13 +1372,13 @@
         <v>2539400000</v>
       </c>
       <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" t="s">
         <v>99</v>
-      </c>
-      <c r="F13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1390,13 +1392,13 @@
         <v>2539380000</v>
       </c>
       <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" t="s">
         <v>101</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>102</v>
-      </c>
-      <c r="G14" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1410,13 +1412,13 @@
         <v>2539390000</v>
       </c>
       <c r="D15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
         <v>104</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>105</v>
-      </c>
-      <c r="G15" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>